<commit_message>
made changes on LED testcase
</commit_message>
<xml_diff>
--- a/TestCases_SATHYA.xlsx
+++ b/TestCases_SATHYA.xlsx
@@ -1,33 +1,111 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\svraman_pc\OneDrive\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB029924-0762-4641-8990-343600CCD902}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00227C06-1722-4C52-A3E5-4DE3A552B194}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="15600" windowHeight="11760" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="1" r:id="rId1"/>
     <sheet name="Refrigerator" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet6" sheetId="6" r:id="rId3"/>
+    <sheet name="Home_kavin" sheetId="7" r:id="rId4"/>
+    <sheet name="LED_kavin" sheetId="8" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>system 5</author>
+  </authors>
+  <commentList>
+    <comment ref="E14" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>system 5:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+1.application spelling error
+5. click on the enter name text field
+6 click on the enter name text field</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E16" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>system 5:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+1.no proper explanation about dropdown
+2. no proper description inexpected results
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E17" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>system 5:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+1.no proper explanation about dropdown
+2. no proper description inexpected results
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="160">
   <si>
     <t>Scope:</t>
   </si>
@@ -661,16 +739,445 @@
   <si>
     <t>SA_HM_3.0</t>
   </si>
+  <si>
+    <t>Testing Home Page in Sathya</t>
+  </si>
+  <si>
+    <t>Home page</t>
+  </si>
+  <si>
+    <t>Kavinkumar</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>03.05.2019</t>
+  </si>
+  <si>
+    <t>Pre-condition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                          Home Page</t>
+  </si>
+  <si>
+    <t>User should open any browser</t>
+  </si>
+  <si>
+    <t>1. Enter the url of the application</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Entered url should be displayed correctly.
+2. Home page should be opened
+</t>
+  </si>
+  <si>
+    <t>Create an account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Launch the URL
+2. Click "Login" button.
+3. Click "Register" button.
+4. Enter your personal details and Choose your gender.
+5. Click enter  "First Name" in the text field.
+6. Click enter  "Last Name " in the text field.
+7. Select "Date of birth" from the drop down.
+8. Click enter "Email" in the text field.
+9. Click enter "Password" in the text field.
+10. Click enter  "Confirm password" in the text field.
+11. Click enter "Company name" in the text field.
+12. Click enter "Phone number" in the text field.
+13. Click "Register" button.
+</t>
+  </si>
+  <si>
+    <t>1. URL should be opened.
+2. Login page should be opened.
+3. Registeration page should be opened.
+4. Gender should be choosed.
+5. The entered text should be displayed.
+6. The entered text should be displayed.
+7. Date of birth should be displayed.
+8. The entered text should be displayed.
+9. The entered text should be displayed.
+10. The entered text should be displayed.
+11. The entered text should be displayed.
+12. The entered phone number should be displayed.
+13. Registered succesfully message should be displayed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                         Login Page</t>
+  </si>
+  <si>
+    <t>1. Open URL of the application.
+2. Click "Login" button
+3. Enter valid "Email ID" in Enter email field.
+4. Enter valid "Password" in the password field.
+5. Click "Login" button.</t>
+  </si>
+  <si>
+    <t>1. URL should be opened.
+2. Login page should be opened.
+4. Email should displayed
+5. Password shoulds be displayed with "*).
+6. My account page should be displayed.</t>
+  </si>
+  <si>
+    <t>SA_HM_3.1</t>
+  </si>
+  <si>
+    <t>1. Open URL of the application.
+2. Click "Login" option
+3. Enter invalid "Email ID" in Enter email field.
+4. Enter valid "Password" in the password field.
+5. Click "Login" button.</t>
+  </si>
+  <si>
+    <t>1. URL should be opened.
+2. Login page should be opened.
+3. Email should displayed
+4. Password shoulds be displayed with "*).
+5. Error message should displayed as "Login was unsuccessful. Please correct the errors and try again".</t>
+  </si>
+  <si>
+    <t>Usability</t>
+  </si>
+  <si>
+    <t>SA_HM_4.0</t>
+  </si>
+  <si>
+    <t>1. Enter the URL of the application.
+2. Place the cursor on the all modules in the home page and click on all modules
+    Home Appliances
+    Audio and Video
+    Electronics
+    Security Solutions
+    Gift Card
+    Offer Zone
+    Featured Products
+    Top Brands
+    Recently Viewed products
+    Informations
+    Service
+    Company
+    Subscribe to Newsletters
+3. Click on facebook icon and check links not broken.
+4. Click on twitter icon and check links not broken.
+5. Click on youtube icon and check links not broken.
+6. Check Webpage contents correct without grammar errors and texts are aligned correct.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. The homepage should opened.
+2. All modules in the home page should highlighted and after click all modules should redirect correctly.
+3. facebook link of application page should opened.
+4. twitter linkof application page should be opened.
+5. youtube link of application should be opened.
+6. No grammar errors and texts are aligned correct.
+</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                                          </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="8" tint="-0.499984740745262"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Note : Positive test scripts are marked in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="8" tint="-0.499984740745262"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>blue</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="8" tint="-0.499984740745262"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                                               </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="8" tint="-0.499984740745262"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Negative test scripts are marked in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="8" tint="-0.499984740745262"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>red</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="8" tint="-0.499984740745262"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Testing Audio and Video Module in Sathya</t>
+  </si>
+  <si>
+    <t>To select and view LED Television in Audio and Video Module</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Audio and Video</t>
+  </si>
+  <si>
+    <t>SA_AV_1.0</t>
+  </si>
+  <si>
+    <t>1)Open URL of the application.
+2)Click on "Audio and Video" drop down.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1)URL should be opened.
+2)Audio and Video dropdown should be displayed with following 
+LED Television
+  HD Ready
+  Full HD
+  Ultra HD
+Home Theatre
+Play Station
+DVD Player
+Fire TV Stick
+Echo and Alexa
+Projector
+Blue Ray Player
+</t>
+  </si>
+  <si>
+    <t>SA_AV_1.1</t>
+  </si>
+  <si>
+    <t>1)Open URL of the application.
+2)Click on "Audio and Video" drop down.
+3)Click on "LED Television" drop down.</t>
+  </si>
+  <si>
+    <t>1)URL should be opened.
+2)Audio and Video dropdown should be displayed with following 
+LED Television
+  HD Ready
+  Full HD
+  Ultra HD
+Home Theatre
+Play Station
+DVD Player
+Fire TV Stick
+Echo and Alexa
+Projector
+Blue Ray Player
+3)"LED Television" drop down should be displayed with following models.
+HD Ready
+Full HD
+Ultra HD</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> HD Ready</t>
+  </si>
+  <si>
+    <t>SA_AV_2.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1)Open URL of an application.
+2)Click on "Audio and Video" drop down.
+3)Click on "LED Television" drop down.
+4)Click on "HD Ready" model from LED Television.
+5)Click on any product.
+6)Click on Features
+7)Click on Review
+</t>
+  </si>
+  <si>
+    <t>1)URL should be opened.
+2)Audio and Video dropdown should be displayed with following 
+LED Television
+  HD Ready
+  Full HD
+  Ultra HD
+Home Theatre
+Play Station
+DVD Player
+Fire TV Stick
+Echo and Alexa
+Projector
+Blue Ray Player
+3)"LED Television" drop down should be displayed with following models.
+HD Ready
+Full HD
+Ultra HD
+4)The selected "HD Ready" model televisions should be displayed.
+5)The selected product should be displayed with its price and description.
+6)The selected product features should be displayed.
+7)The available product reviews should displayed.</t>
+  </si>
+  <si>
+    <t>SA_AV_2.1</t>
+  </si>
+  <si>
+    <t>User visited "Product Page".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Click on Product Image.
+2.Click on number of Products "+" Button.
+3.Click on number of Products "-" Button.
+4.Click on "Add to cart" button.
+5.Click on "Check out" Button.
+6.Click on "Go to cart" button.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Corresponding Product Images should be opened in new page.
+2.Total number of products should be increased by 1.
+ 3.Total number of products should be decreased by 1.
+4. "Add to Cart" Page should be opened with following details.
+"The Product has been added successfully" message should be shown.
+Product name, Price, Number of Proucts, Sub Total should be displayed with corresponding details.
+Move to "Wish list" button.
+"Delete" Button
+"Go to Cart" button.
+"Check out" button.
+5.Sign In Page should be opened.
+6.Shopping Cart page should be opened with following details.
+Product name
+Product Price
+Product Quantity
+Sub Total
+Shipping Chagres
+Tax
+Total
+"Contine shopping" as button.
+"Check out" as button.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Full HD</t>
+  </si>
+  <si>
+    <t>SA_AV_3.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1)Open URL of an application.
+2)Click on "Audio and Video" drop down.
+3)Click on "LED Television" drop down.
+4)Click on "Full HD" model from LED Television.
+5)Click on any product.
+6)Click on Features
+7)Click on Review
+</t>
+  </si>
+  <si>
+    <t>1)URL should be opened.
+2)Audio and Video dropdown should be displayed with following 
+LED Television
+  HD Ready
+  Full HD
+  Ultra HD
+Home Theatre
+Play Station
+DVD Player
+Fire TV Stick
+Echo and Alexa
+Projector
+Blue Ray Player
+3)"LED Television" drop down should be displayed with following models.
+HD Ready
+Full HD
+Ultra HD
+4)The selected "Full HD" model televisions should be displayed.
+5)The selected product should be displayed with its price and description.
+6)The selected product features should be displayed.
+7)The available product reviews should displayed.</t>
+  </si>
+  <si>
+    <t>SA_AV_3.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ultra HD</t>
+  </si>
+  <si>
+    <t>SA_AV_4.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1)Open URL of an application.
+2)Click on "Audio and Video" drop down.
+3)Click on "LED Television" drop down.
+4)Click on "Ultra HD" model from LED Television.
+5)Click on any product.
+6)Click on Features
+7)Click on Review
+</t>
+  </si>
+  <si>
+    <t>1)URL should be opened.
+2)Audio and Video dropdown should be displayed with following 
+LED Television
+  HD Ready
+  Full HD
+  Ultra HD
+Home Theatre
+Play Station
+DVD Player
+Fire TV Stick
+Echo and Alexa
+Projector
+Blue Ray Player
+3)"LED Television" drop down should be displayed with following models.
+HD Ready
+Full HD
+Ultra HD
+4)The selected "Ultra HD" model televisions should be displayed.
+5)The selected product should be displayed with its price and description.
+6)The selected product features should be displayed.
+7)The available product reviews should displayed.</t>
+  </si>
+  <si>
+    <t>SA_AV_4.1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="d\ mmm\ yy"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -713,8 +1220,59 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="8" tint="-0.499984740745262"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="8" tint="-0.499984740745262"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="8" tint="-0.499984740745262"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="8" tint="-0.499984740745262"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="8" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -751,8 +1309,38 @@
         <bgColor indexed="31"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="54"/>
+        <bgColor indexed="23"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="23"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+        <bgColor indexed="34"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -827,12 +1415,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -874,12 +1478,224 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="8" fillId="10" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="11" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{01201A5F-C506-4699-8884-1BF5B0DEFE84}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="30"/>
+          <bgColor indexed="48"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color indexed="9"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="21"/>
+          <bgColor indexed="57"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="30"/>
+          <bgColor indexed="48"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color indexed="13"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="60"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color indexed="9"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="21"/>
+          <bgColor indexed="57"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -935,7 +1751,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -987,7 +1803,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1181,31 +1997,31 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D457729A-249C-40D9-B7AA-1752B0EFEAF7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" customWidth="1"/>
-    <col min="2" max="2" width="38.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.88671875" customWidth="1"/>
-    <col min="4" max="4" width="32.5546875" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="32.5703125" customWidth="1"/>
     <col min="5" max="5" width="39" customWidth="1"/>
-    <col min="6" max="6" width="16.77734375" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1220,7 +2036,7 @@
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
     </row>
-    <row r="2" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="15.75">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1235,7 +2051,7 @@
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="15.75">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1250,7 +2066,7 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="31.5">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1263,7 +2079,7 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="15.75">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1276,7 +2092,7 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:9" ht="31.8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="15.75">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1289,7 +2105,7 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="15.75">
       <c r="A7" s="6"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -1300,7 +2116,7 @@
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
     </row>
-    <row r="8" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="31.5">
       <c r="A8" s="8" t="s">
         <v>7</v>
       </c>
@@ -1329,7 +2145,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="15.75">
       <c r="A9" s="12" t="s">
         <v>21</v>
       </c>
@@ -1342,7 +2158,7 @@
       <c r="H9" s="12"/>
       <c r="I9" s="14"/>
     </row>
-    <row r="10" spans="1:9" ht="221.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="221.45" customHeight="1">
       <c r="A10" s="9" t="s">
         <v>19</v>
       </c>
@@ -1359,7 +2175,7 @@
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
     </row>
-    <row r="11" spans="1:9" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="77.45" customHeight="1">
       <c r="A11" s="9" t="s">
         <v>93</v>
       </c>
@@ -1376,7 +2192,7 @@
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
     </row>
-    <row r="12" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="75" customHeight="1">
       <c r="A12" s="9" t="s">
         <v>98</v>
       </c>
@@ -1393,7 +2209,7 @@
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
     </row>
-    <row r="13" spans="1:9" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="46.9" customHeight="1">
       <c r="A13" s="9" t="s">
         <v>99</v>
       </c>
@@ -1410,7 +2226,7 @@
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
     </row>
-    <row r="14" spans="1:9" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="94.5">
       <c r="A14" s="9" t="s">
         <v>102</v>
       </c>
@@ -1427,7 +2243,7 @@
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
     </row>
-    <row r="15" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="31.5">
       <c r="A15" s="9" t="s">
         <v>107</v>
       </c>
@@ -1444,7 +2260,7 @@
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
     </row>
-    <row r="16" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="15.75">
       <c r="A16" s="9"/>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
@@ -1455,7 +2271,7 @@
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
     </row>
-    <row r="17" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="15.75">
       <c r="A17" s="12" t="s">
         <v>18</v>
       </c>
@@ -1468,7 +2284,7 @@
       <c r="H17" s="12"/>
       <c r="I17" s="13"/>
     </row>
-    <row r="18" spans="1:9" ht="76.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="76.150000000000006" customHeight="1">
       <c r="A18" s="9" t="s">
         <v>19</v>
       </c>
@@ -1485,7 +2301,7 @@
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
     </row>
-    <row r="19" spans="1:9" ht="187.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="187.15" customHeight="1">
       <c r="A19" s="9" t="s">
         <v>93</v>
       </c>
@@ -1502,7 +2318,7 @@
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
     </row>
-    <row r="20" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="15.75">
       <c r="A20" s="9"/>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
@@ -1513,7 +2329,7 @@
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
     </row>
-    <row r="21" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="15.75">
       <c r="A21" s="9"/>
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
@@ -1524,7 +2340,7 @@
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
     </row>
-    <row r="22" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="15.75">
       <c r="A22" s="9"/>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
@@ -1535,7 +2351,7 @@
       <c r="H22" s="10"/>
       <c r="I22" s="10"/>
     </row>
-    <row r="23" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="15.75">
       <c r="A23" s="9"/>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
@@ -1546,7 +2362,7 @@
       <c r="H23" s="10"/>
       <c r="I23" s="10"/>
     </row>
-    <row r="24" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="15.75">
       <c r="A24" s="9"/>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
@@ -1557,7 +2373,7 @@
       <c r="H24" s="10"/>
       <c r="I24" s="10"/>
     </row>
-    <row r="25" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="15.75">
       <c r="A25" s="9"/>
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
@@ -1568,7 +2384,7 @@
       <c r="H25" s="10"/>
       <c r="I25" s="10"/>
     </row>
-    <row r="26" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="15.75">
       <c r="A26" s="9"/>
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
@@ -1579,7 +2395,7 @@
       <c r="H26" s="10"/>
       <c r="I26" s="10"/>
     </row>
-    <row r="27" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="15.75">
       <c r="A27" s="9"/>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
@@ -1590,7 +2406,7 @@
       <c r="H27" s="10"/>
       <c r="I27" s="10"/>
     </row>
-    <row r="28" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="15.75">
       <c r="A28" s="9"/>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
@@ -1601,7 +2417,7 @@
       <c r="H28" s="10"/>
       <c r="I28" s="10"/>
     </row>
-    <row r="29" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="15.75">
       <c r="A29" s="9"/>
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
@@ -1612,7 +2428,7 @@
       <c r="H29" s="10"/>
       <c r="I29" s="10"/>
     </row>
-    <row r="30" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="15.75">
       <c r="A30" s="9"/>
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
@@ -1623,7 +2439,7 @@
       <c r="H30" s="10"/>
       <c r="I30" s="10"/>
     </row>
-    <row r="31" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="15.75">
       <c r="A31" s="9"/>
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
@@ -1634,7 +2450,7 @@
       <c r="H31" s="10"/>
       <c r="I31" s="10"/>
     </row>
-    <row r="32" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="15.75">
       <c r="A32" s="9"/>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
@@ -1656,24 +2472,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A108459D-E0CE-4616-9E1B-82332EB0213C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
-    <col min="2" max="2" width="41.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5546875" customWidth="1"/>
-    <col min="4" max="4" width="33.33203125" customWidth="1"/>
-    <col min="5" max="5" width="44.33203125" customWidth="1"/>
-    <col min="6" max="6" width="21.77734375" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="41.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" customWidth="1"/>
+    <col min="4" max="4" width="33.28515625" customWidth="1"/>
+    <col min="5" max="5" width="44.28515625" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1688,7 +2504,7 @@
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
     </row>
-    <row r="2" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="15.75">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1703,7 +2519,7 @@
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="15.75">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1718,7 +2534,7 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="15.75">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1731,7 +2547,7 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="15.75">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1744,7 +2560,7 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:9" ht="31.8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="15.75">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1757,7 +2573,7 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="15.75">
       <c r="A7" s="6"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -1768,7 +2584,7 @@
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
     </row>
-    <row r="8" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="31.5">
       <c r="A8" s="8" t="s">
         <v>7</v>
       </c>
@@ -1797,7 +2613,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="15.75">
       <c r="A9" s="12" t="s">
         <v>28</v>
       </c>
@@ -1810,7 +2626,7 @@
       <c r="H9" s="12"/>
       <c r="I9" s="13"/>
     </row>
-    <row r="10" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="409.5">
       <c r="A10" s="9" t="s">
         <v>27</v>
       </c>
@@ -1829,7 +2645,7 @@
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
     </row>
-    <row r="11" spans="1:9" ht="132" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="132" customHeight="1">
       <c r="A11" s="9" t="s">
         <v>43</v>
       </c>
@@ -1846,7 +2662,7 @@
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
     </row>
-    <row r="12" spans="1:9" ht="130.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="130.15" customHeight="1">
       <c r="A12" s="9" t="s">
         <v>46</v>
       </c>
@@ -1863,7 +2679,7 @@
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
     </row>
-    <row r="13" spans="1:9" ht="130.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="130.15" customHeight="1">
       <c r="A13" s="9" t="s">
         <v>49</v>
       </c>
@@ -1880,7 +2696,7 @@
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
     </row>
-    <row r="14" spans="1:9" ht="130.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="130.15" customHeight="1">
       <c r="A14" s="9" t="s">
         <v>51</v>
       </c>
@@ -1897,7 +2713,7 @@
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
     </row>
-    <row r="15" spans="1:9" ht="78" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="78" customHeight="1">
       <c r="A15" s="9" t="s">
         <v>55</v>
       </c>
@@ -1914,7 +2730,7 @@
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
     </row>
-    <row r="16" spans="1:9" ht="78" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="78" customHeight="1">
       <c r="A16" s="9" t="s">
         <v>58</v>
       </c>
@@ -1931,7 +2747,7 @@
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
     </row>
-    <row r="17" spans="1:9" ht="78" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="78" customHeight="1">
       <c r="A17" s="9" t="s">
         <v>61</v>
       </c>
@@ -1948,7 +2764,7 @@
       <c r="H17" s="10"/>
       <c r="I17" s="10"/>
     </row>
-    <row r="18" spans="1:9" ht="78" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="78" customHeight="1">
       <c r="A18" s="9" t="s">
         <v>65</v>
       </c>
@@ -1967,7 +2783,7 @@
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
     </row>
-    <row r="19" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="15.75">
       <c r="A19" s="12" t="s">
         <v>35</v>
       </c>
@@ -1980,7 +2796,7 @@
       <c r="H19" s="12"/>
       <c r="I19" s="13"/>
     </row>
-    <row r="20" spans="1:9" ht="175.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="175.15" customHeight="1">
       <c r="A20" s="9" t="s">
         <v>31</v>
       </c>
@@ -1999,7 +2815,7 @@
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
     </row>
-    <row r="21" spans="1:9" ht="108" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="108" customHeight="1">
       <c r="A21" s="9" t="s">
         <v>37</v>
       </c>
@@ -2016,7 +2832,7 @@
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
     </row>
-    <row r="22" spans="1:9" ht="76.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="76.150000000000006" customHeight="1">
       <c r="A22" s="9" t="s">
         <v>40</v>
       </c>
@@ -2033,7 +2849,7 @@
       <c r="H22" s="10"/>
       <c r="I22" s="10"/>
     </row>
-    <row r="23" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="15.75">
       <c r="A23" s="12" t="s">
         <v>66</v>
       </c>
@@ -2046,7 +2862,7 @@
       <c r="H23" s="12"/>
       <c r="I23" s="13"/>
     </row>
-    <row r="24" spans="1:9" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="69.599999999999994" customHeight="1">
       <c r="A24" s="9" t="s">
         <v>72</v>
       </c>
@@ -2065,7 +2881,7 @@
       <c r="H24" s="10"/>
       <c r="I24" s="10"/>
     </row>
-    <row r="25" spans="1:9" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="69.599999999999994" customHeight="1">
       <c r="A25" s="9" t="s">
         <v>73</v>
       </c>
@@ -2082,7 +2898,7 @@
       <c r="H25" s="10"/>
       <c r="I25" s="10"/>
     </row>
-    <row r="26" spans="1:9" ht="78" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="78.75">
       <c r="A26" s="9" t="s">
         <v>74</v>
       </c>
@@ -2099,7 +2915,7 @@
       <c r="H26" s="10"/>
       <c r="I26" s="10"/>
     </row>
-    <row r="27" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="15.75">
       <c r="A27" s="12" t="s">
         <v>69</v>
       </c>
@@ -2112,7 +2928,7 @@
       <c r="H27" s="12"/>
       <c r="I27" s="13"/>
     </row>
-    <row r="28" spans="1:9" ht="140.4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="141.75">
       <c r="A28" s="9" t="s">
         <v>75</v>
       </c>
@@ -2131,7 +2947,7 @@
       <c r="H28" s="10"/>
       <c r="I28" s="10"/>
     </row>
-    <row r="29" spans="1:9" ht="312" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="315">
       <c r="A29" s="9" t="s">
         <v>76</v>
       </c>
@@ -2148,7 +2964,7 @@
       <c r="H29" s="10"/>
       <c r="I29" s="10"/>
     </row>
-    <row r="30" spans="1:9" ht="78" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="78.75">
       <c r="A30" s="9" t="s">
         <v>77</v>
       </c>
@@ -2165,7 +2981,7 @@
       <c r="H30" s="10"/>
       <c r="I30" s="10"/>
     </row>
-    <row r="31" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="15.75">
       <c r="A31" s="12" t="s">
         <v>78</v>
       </c>
@@ -2178,7 +2994,7 @@
       <c r="H31" s="12"/>
       <c r="I31" s="13"/>
     </row>
-    <row r="32" spans="1:9" ht="140.4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="141.75">
       <c r="A32" s="9" t="s">
         <v>81</v>
       </c>
@@ -2197,7 +3013,7 @@
       <c r="H32" s="10"/>
       <c r="I32" s="10"/>
     </row>
-    <row r="33" spans="1:9" ht="312" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="315">
       <c r="A33" s="9" t="s">
         <v>82</v>
       </c>
@@ -2214,7 +3030,7 @@
       <c r="H33" s="10"/>
       <c r="I33" s="10"/>
     </row>
-    <row r="34" spans="1:9" ht="78" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="78.75">
       <c r="A34" s="9" t="s">
         <v>83</v>
       </c>
@@ -2231,7 +3047,7 @@
       <c r="H34" s="10"/>
       <c r="I34" s="10"/>
     </row>
-    <row r="35" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" ht="15.75">
       <c r="A35" s="12" t="s">
         <v>87</v>
       </c>
@@ -2244,7 +3060,7 @@
       <c r="H35" s="12"/>
       <c r="I35" s="13"/>
     </row>
-    <row r="36" spans="1:9" ht="140.4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="141.75">
       <c r="A36" s="9" t="s">
         <v>84</v>
       </c>
@@ -2263,7 +3079,7 @@
       <c r="H36" s="10"/>
       <c r="I36" s="10"/>
     </row>
-    <row r="37" spans="1:9" ht="312" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" ht="315">
       <c r="A37" s="9" t="s">
         <v>85</v>
       </c>
@@ -2280,7 +3096,7 @@
       <c r="H37" s="10"/>
       <c r="I37" s="10"/>
     </row>
-    <row r="38" spans="1:9" ht="78" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" ht="78.75">
       <c r="A38" s="9" t="s">
         <v>86</v>
       </c>
@@ -2297,7 +3113,7 @@
       <c r="H38" s="10"/>
       <c r="I38" s="10"/>
     </row>
-    <row r="39" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" ht="15.75">
       <c r="A39" s="9"/>
       <c r="B39" s="10"/>
       <c r="C39" s="10"/>
@@ -2308,7 +3124,7 @@
       <c r="H39" s="10"/>
       <c r="I39" s="10"/>
     </row>
-    <row r="40" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" ht="15.75">
       <c r="A40" s="9"/>
       <c r="B40" s="10"/>
       <c r="C40" s="10"/>
@@ -2319,7 +3135,7 @@
       <c r="H40" s="10"/>
       <c r="I40" s="10"/>
     </row>
-    <row r="41" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" ht="15.75">
       <c r="A41" s="9"/>
       <c r="B41" s="10"/>
       <c r="C41" s="10"/>
@@ -2330,7 +3146,7 @@
       <c r="H41" s="10"/>
       <c r="I41" s="10"/>
     </row>
-    <row r="42" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" ht="15.75">
       <c r="A42" s="9"/>
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
@@ -2356,22 +3172,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07937DB0-3E7E-457C-B596-44C4579C993D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1"/>
-    <col min="3" max="3" width="17.88671875" customWidth="1"/>
-    <col min="4" max="4" width="23.5546875" customWidth="1"/>
-    <col min="5" max="5" width="29.77734375" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" customWidth="1"/>
+    <col min="5" max="5" width="29.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15.75">
       <c r="A1" s="12" t="s">
         <v>87</v>
       </c>
@@ -2384,7 +3200,7 @@
       <c r="H1" s="12"/>
       <c r="I1" s="13"/>
     </row>
-    <row r="2" spans="1:9" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="189">
       <c r="A2" s="9" t="s">
         <v>84</v>
       </c>
@@ -2403,7 +3219,7 @@
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
     </row>
-    <row r="3" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="409.5">
       <c r="A3" s="9" t="s">
         <v>85</v>
       </c>
@@ -2420,7 +3236,7 @@
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
     </row>
-    <row r="4" spans="1:9" ht="374.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="94.5">
       <c r="A4" s="9" t="s">
         <v>86</v>
       </c>
@@ -2443,4 +3259,704 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" style="39" customWidth="1"/>
+    <col min="2" max="2" width="37.7109375" style="39" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="39" customWidth="1"/>
+    <col min="4" max="4" width="119.5703125" style="39" customWidth="1"/>
+    <col min="5" max="5" width="101.42578125" style="39" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="39"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="17" customFormat="1">
+      <c r="A1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16">
+        <v>0</v>
+      </c>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+    </row>
+    <row r="2" spans="1:10" s="22" customFormat="1">
+      <c r="A2" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+    </row>
+    <row r="3" spans="1:10" s="26" customFormat="1">
+      <c r="A3" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="24"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+    </row>
+    <row r="4" spans="1:10" s="26" customFormat="1">
+      <c r="A4" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" s="24"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+    </row>
+    <row r="5" spans="1:10" s="26" customFormat="1" ht="31.5">
+      <c r="A5" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="19"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+    </row>
+    <row r="6" spans="1:10" s="26" customFormat="1">
+      <c r="A6" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6" s="28"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+    </row>
+    <row r="7" spans="1:10" s="26" customFormat="1">
+      <c r="A7" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="C7" s="28"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+    </row>
+    <row r="8" spans="1:10" s="17" customFormat="1">
+      <c r="A8" s="15"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+    </row>
+    <row r="9" spans="1:10" s="26" customFormat="1">
+      <c r="A9" s="30"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+    </row>
+    <row r="10" spans="1:10" s="26" customFormat="1" ht="31.5">
+      <c r="A10" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="D10" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="31" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="33" customFormat="1">
+      <c r="A11" s="32" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+    </row>
+    <row r="12" spans="1:10" ht="47.25">
+      <c r="A12" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="35"/>
+      <c r="C12" s="36" t="s">
+        <v>115</v>
+      </c>
+      <c r="D12" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="E12" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="F12" s="35"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="36"/>
+    </row>
+    <row r="13" spans="1:10" s="46" customFormat="1">
+      <c r="A13" s="40"/>
+      <c r="B13" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="C13" s="42"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
+    </row>
+    <row r="14" spans="1:10" s="33" customFormat="1" ht="202.5" customHeight="1">
+      <c r="A14" s="47" t="s">
+        <v>93</v>
+      </c>
+      <c r="B14" s="48"/>
+      <c r="C14" s="48"/>
+      <c r="D14" s="49" t="s">
+        <v>119</v>
+      </c>
+      <c r="E14" s="50" t="s">
+        <v>120</v>
+      </c>
+      <c r="F14" s="48"/>
+      <c r="G14" s="48"/>
+      <c r="H14" s="48"/>
+      <c r="I14" s="48"/>
+    </row>
+    <row r="15" spans="1:10" s="26" customFormat="1">
+      <c r="A15" s="51" t="s">
+        <v>121</v>
+      </c>
+      <c r="B15" s="51"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="51"/>
+      <c r="G15" s="51"/>
+      <c r="H15" s="51"/>
+      <c r="I15" s="51"/>
+    </row>
+    <row r="16" spans="1:10" ht="78.75">
+      <c r="A16" s="47" t="s">
+        <v>107</v>
+      </c>
+      <c r="B16" s="48"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="52" t="s">
+        <v>122</v>
+      </c>
+      <c r="E16" s="52" t="s">
+        <v>123</v>
+      </c>
+      <c r="F16" s="48"/>
+      <c r="G16" s="48"/>
+      <c r="H16" s="48"/>
+      <c r="I16" s="48"/>
+      <c r="J16" s="33"/>
+    </row>
+    <row r="17" spans="1:9" ht="78.75">
+      <c r="A17" s="47" t="s">
+        <v>124</v>
+      </c>
+      <c r="B17" s="35"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="52" t="s">
+        <v>125</v>
+      </c>
+      <c r="E17" s="52" t="s">
+        <v>126</v>
+      </c>
+      <c r="F17" s="35"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="36"/>
+    </row>
+    <row r="18" spans="1:9" s="46" customFormat="1">
+      <c r="A18" s="40" t="s">
+        <v>127</v>
+      </c>
+      <c r="B18" s="43"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+    </row>
+    <row r="19" spans="1:9" s="22" customFormat="1" ht="387.75" customHeight="1">
+      <c r="A19" s="47" t="s">
+        <v>128</v>
+      </c>
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="E19" s="35" t="s">
+        <v>130</v>
+      </c>
+      <c r="F19" s="35"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="36"/>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="53" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="53" t="s">
+        <v>132</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A11:I11"/>
+    <mergeCell ref="A15:I15"/>
+  </mergeCells>
+  <conditionalFormatting sqref="G15">
+    <cfRule type="cellIs" dxfId="5" priority="1" stopIfTrue="1" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"Block"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" style="54" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" style="54" customWidth="1"/>
+    <col min="3" max="3" width="29.42578125" style="54" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" style="54" customWidth="1"/>
+    <col min="5" max="5" width="37.7109375" style="54" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="54"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16">
+        <v>0</v>
+      </c>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+    </row>
+    <row r="3" spans="1:9" ht="23.1" customHeight="1">
+      <c r="A3" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="C3" s="24"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+    </row>
+    <row r="4" spans="1:9" ht="27.95" customHeight="1">
+      <c r="A4" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" s="20"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+    </row>
+    <row r="5" spans="1:9" ht="31.5">
+      <c r="A5" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="19"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="55" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6" s="56"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+    </row>
+    <row r="7" spans="1:9" ht="31.5">
+      <c r="A7" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="57" t="s">
+        <v>112</v>
+      </c>
+      <c r="C7" s="56"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="15"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="58"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+    </row>
+    <row r="10" spans="1:9" ht="35.1" customHeight="1">
+      <c r="A10" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="D10" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="31" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="40"/>
+      <c r="B11" s="41" t="s">
+        <v>135</v>
+      </c>
+      <c r="C11" s="42"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+    </row>
+    <row r="12" spans="1:9" ht="267.75">
+      <c r="A12" s="59" t="s">
+        <v>136</v>
+      </c>
+      <c r="B12" s="60"/>
+      <c r="C12" s="36" t="s">
+        <v>115</v>
+      </c>
+      <c r="D12" s="61" t="s">
+        <v>137</v>
+      </c>
+      <c r="E12" s="61" t="s">
+        <v>138</v>
+      </c>
+      <c r="F12" s="61"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="60"/>
+      <c r="I12" s="60"/>
+    </row>
+    <row r="13" spans="1:9" ht="330.75">
+      <c r="A13" s="59" t="s">
+        <v>139</v>
+      </c>
+      <c r="B13" s="60"/>
+      <c r="C13" s="60"/>
+      <c r="D13" s="61" t="s">
+        <v>140</v>
+      </c>
+      <c r="E13" s="61" t="s">
+        <v>141</v>
+      </c>
+      <c r="F13" s="61"/>
+      <c r="G13" s="60"/>
+      <c r="H13" s="60"/>
+      <c r="I13" s="60"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="40"/>
+      <c r="B14" s="41" t="s">
+        <v>142</v>
+      </c>
+      <c r="C14" s="42"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="42"/>
+    </row>
+    <row r="15" spans="1:9" ht="409.5">
+      <c r="A15" s="59" t="s">
+        <v>143</v>
+      </c>
+      <c r="B15" s="60"/>
+      <c r="C15" s="60"/>
+      <c r="D15" s="61" t="s">
+        <v>144</v>
+      </c>
+      <c r="E15" s="61" t="s">
+        <v>145</v>
+      </c>
+      <c r="F15" s="61"/>
+      <c r="G15" s="60"/>
+      <c r="H15" s="60"/>
+      <c r="I15" s="60"/>
+    </row>
+    <row r="16" spans="1:9" ht="409.5">
+      <c r="A16" s="59" t="s">
+        <v>146</v>
+      </c>
+      <c r="B16" s="60"/>
+      <c r="C16" s="62" t="s">
+        <v>147</v>
+      </c>
+      <c r="D16" s="63" t="s">
+        <v>148</v>
+      </c>
+      <c r="E16" s="64" t="s">
+        <v>149</v>
+      </c>
+      <c r="F16" s="61"/>
+      <c r="G16" s="60"/>
+      <c r="H16" s="60"/>
+      <c r="I16" s="60"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="40"/>
+      <c r="B17" s="41" t="s">
+        <v>150</v>
+      </c>
+      <c r="C17" s="42"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+    </row>
+    <row r="18" spans="1:9" ht="409.5">
+      <c r="A18" s="59" t="s">
+        <v>151</v>
+      </c>
+      <c r="D18" s="61" t="s">
+        <v>152</v>
+      </c>
+      <c r="E18" s="61" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="409.5">
+      <c r="A19" s="59" t="s">
+        <v>154</v>
+      </c>
+      <c r="B19" s="60"/>
+      <c r="C19" s="62" t="s">
+        <v>147</v>
+      </c>
+      <c r="D19" s="63" t="s">
+        <v>148</v>
+      </c>
+      <c r="E19" s="64" t="s">
+        <v>149</v>
+      </c>
+      <c r="F19" s="61"/>
+      <c r="G19" s="60"/>
+      <c r="H19" s="60"/>
+      <c r="I19" s="60"/>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="40"/>
+      <c r="B20" s="41" t="s">
+        <v>155</v>
+      </c>
+      <c r="C20" s="42"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="45"/>
+      <c r="H20" s="42"/>
+      <c r="I20" s="42"/>
+    </row>
+    <row r="21" spans="1:9" ht="409.5">
+      <c r="A21" s="59" t="s">
+        <v>156</v>
+      </c>
+      <c r="D21" s="61" t="s">
+        <v>157</v>
+      </c>
+      <c r="E21" s="61" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="409.5">
+      <c r="A22" s="59" t="s">
+        <v>159</v>
+      </c>
+      <c r="B22" s="60"/>
+      <c r="C22" s="62" t="s">
+        <v>147</v>
+      </c>
+      <c r="D22" s="63" t="s">
+        <v>148</v>
+      </c>
+      <c r="E22" s="64" t="s">
+        <v>149</v>
+      </c>
+      <c r="F22" s="61"/>
+      <c r="G22" s="60"/>
+      <c r="H22" s="60"/>
+      <c r="I22" s="60"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>